<commit_message>
Updated with results for Generator1
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tester" sheetId="1" r:id="rId1"/>
+    <sheet name="Generator1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Tester</t>
   </si>
@@ -55,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,6 +78,21 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -112,12 +128,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,13 +157,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,14 +506,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
@@ -488,19 +523,19 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -628,4 +663,166 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="C4" s="3">
+        <v>22576583</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4/1000000000</f>
+        <v>2.2576583000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="C5" s="3">
+        <v>34172763</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5/1000000000</f>
+        <v>3.4172763000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="C6" s="3">
+        <v>18576956</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D10" si="0">C6/1000000000</f>
+        <v>1.8576955999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="C7" s="3">
+        <v>16244818</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6244818000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5">
+        <v>18095574</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8095574E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <f>AVERAGE(C4:C8)</f>
+        <v>21933338.800000001</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>2.19333388E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <f>C9/7776</f>
+        <v>2820.6454218106996</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.8206454218106995E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="2">
+        <f>55^33</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="C13" s="3">
+        <f>B13*C10</f>
+        <v>7.6263590582300777E+60</v>
+      </c>
+      <c r="D13" s="3">
+        <f>D10*B13</f>
+        <v>7.626359058230078E+51</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13/(60*60)</f>
+        <v>2.1184330717305773E+48</v>
+      </c>
+      <c r="F13" s="2">
+        <f>E13/24</f>
+        <v>8.8268044655440716E+46</v>
+      </c>
+      <c r="G13" s="2">
+        <f>F13/365</f>
+        <v>2.4183025932997458E+44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added results for Generator2 optimizations
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tester" sheetId="1" r:id="rId1"/>
     <sheet name="Generator1" sheetId="2" r:id="rId2"/>
+    <sheet name="Generator2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Tester</t>
   </si>
@@ -50,6 +51,24 @@
   </si>
   <si>
     <t>[year]</t>
+  </si>
+  <si>
+    <t>4 channels, 5 comparators: 5346 networks</t>
+  </si>
+  <si>
+    <t>1 network (7776):</t>
+  </si>
+  <si>
+    <t>1 network (5346):</t>
+  </si>
+  <si>
+    <t>zonder parallele varianten  (1,2)(3,4) en (3,4)(1,2)</t>
+  </si>
+  <si>
+    <t>1 network (2376):</t>
+  </si>
+  <si>
+    <t>zonder dubbels (1,2)(1,2)</t>
   </si>
 </sst>
 </file>
@@ -96,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,7 +153,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,8 +165,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,24 +188,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,28 +561,28 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="3">
@@ -619,10 +657,10 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="2">
@@ -669,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -685,28 +723,28 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="3">
@@ -781,10 +819,10 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:7">
@@ -825,4 +863,383 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="C4" s="3">
+        <v>18724058</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4/1000000000</f>
+        <v>1.8724057999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="C5" s="3">
+        <v>25851937</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5/1000000000</f>
+        <v>2.5851936999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="C6" s="3">
+        <v>17988546</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D11" si="0">C6/1000000000</f>
+        <v>1.7988546000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="C7" s="3">
+        <v>19676560</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9676559999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5">
+        <v>15555244</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5555243999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <f>AVERAGE(C4:C8)</f>
+        <v>19559269</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9559269000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
+        <f>C9/7776</f>
+        <v>2515.3380915637858</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5153380915637856E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <f>C9/5346</f>
+        <v>3658.6735877291435</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.6586735877291436E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="2">
+        <f>55^33</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="C14" s="3">
+        <f>B14*C10</f>
+        <v>6.8008801428129461E+60</v>
+      </c>
+      <c r="D14" s="3">
+        <f>D10*B14</f>
+        <v>6.8008801428129466E+51</v>
+      </c>
+      <c r="E14" s="2">
+        <f>D14/(60*60)</f>
+        <v>1.8891333730035963E+48</v>
+      </c>
+      <c r="F14" s="2">
+        <f>E14/24</f>
+        <v>7.8713890541816516E+46</v>
+      </c>
+      <c r="G14" s="2">
+        <f>F14/365</f>
+        <v>2.1565449463511374E+44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="C15" s="3">
+        <f>C11*B14</f>
+        <v>9.8921892986370147E+60</v>
+      </c>
+      <c r="D15" s="3">
+        <f>D11*B14</f>
+        <v>9.8921892986370145E+51</v>
+      </c>
+      <c r="E15" s="2">
+        <f>D15/(60*60)</f>
+        <v>2.7478303607325042E+48</v>
+      </c>
+      <c r="F15" s="2">
+        <f>E15/24</f>
+        <v>1.1449293169718767E+47</v>
+      </c>
+      <c r="G15" s="2">
+        <f>F15/365</f>
+        <v>3.1367926492380185E+44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" s="9" customFormat="1"/>
+    <row r="19" spans="2:9">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="C21" s="3">
+        <v>21177397</v>
+      </c>
+      <c r="D21" s="3">
+        <f>C21/1000000000</f>
+        <v>2.1177397000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="C22" s="3">
+        <v>9723433</v>
+      </c>
+      <c r="D22" s="3">
+        <f>C22/1000000000</f>
+        <v>9.7234330000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="C23" s="3">
+        <v>17796970</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" ref="D23:D28" si="1">C23/1000000000</f>
+        <v>1.7796969999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="C24" s="3">
+        <v>21073791</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1073791000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5">
+        <v>18971347</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8971347E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3">
+        <f>AVERAGE(C21:C25)</f>
+        <v>17748587.600000001</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="1"/>
+        <v>1.7748587600000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="3">
+        <f>C26/7776</f>
+        <v>2282.4829732510289</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2824829732510289E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2">
+        <f>C26/2376</f>
+        <v>7469.9442760942766</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="1"/>
+        <v>7.4699442760942768E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="2">
+        <f>55^33</f>
+        <v>2.703763826271497E+57</v>
+      </c>
+      <c r="C31" s="3">
+        <f>B31*C27</f>
+        <v>6.1712948971567445E+60</v>
+      </c>
+      <c r="D31" s="3">
+        <f>D27*B31</f>
+        <v>6.1712948971567455E+51</v>
+      </c>
+      <c r="E31" s="2">
+        <f>D31/(60*60)</f>
+        <v>1.7142485825435405E+48</v>
+      </c>
+      <c r="F31" s="2">
+        <f>E31/24</f>
+        <v>7.1427024272647519E+46</v>
+      </c>
+      <c r="G31" s="2">
+        <f>F31/365</f>
+        <v>1.9569047745930828E+44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="C32" s="3">
+        <f>C28*B31</f>
+        <v>2.0196965117967529E+61</v>
+      </c>
+      <c r="D32" s="3">
+        <f>D28*B31</f>
+        <v>2.0196965117967531E+52</v>
+      </c>
+      <c r="E32" s="2">
+        <f>D32/(60*60)</f>
+        <v>5.610268088324314E+48</v>
+      </c>
+      <c r="F32" s="2">
+        <f>E32/24</f>
+        <v>2.3376117034684643E+47</v>
+      </c>
+      <c r="G32" s="2">
+        <f>F32/365</f>
+        <v>6.4044156259409982E+44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B30:C30"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aanvullen timeTest voor de tester. Uitbereiding van 5 naar 10 tests.
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tester" sheetId="1" r:id="rId1"/>
@@ -75,6 +75,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="176" formatCode="0.00000E+00;\_x0000_"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -153,7 +157,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -171,8 +175,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,8 +205,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="23">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -205,6 +234,9 @@
     <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -213,6 +245,9 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G13"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -578,119 +613,169 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="2:7">
+      <c r="B4" s="8"/>
       <c r="C4" s="3">
+        <v>207773446</v>
+      </c>
+      <c r="D4" s="11">
+        <f>C4/1000000000</f>
+        <v>0.207773446</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="8"/>
+      <c r="C5" s="3">
+        <v>205065950</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" ref="D5:D8" si="0">C5/1000000000</f>
+        <v>0.20506595</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="8"/>
+      <c r="C6" s="3">
+        <v>205841056</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.20584105599999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="8"/>
+      <c r="C7" s="3">
+        <v>214539254</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>0.21453925400000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="8"/>
+      <c r="C8" s="3">
+        <v>214655080</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>0.21465508</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="C9" s="3">
         <v>212575952</v>
       </c>
-      <c r="D4" s="3">
-        <f>C4/1000000000</f>
+      <c r="D9" s="11">
+        <f>C9/1000000000</f>
         <v>0.21257595200000001</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
-      <c r="C5" s="3">
+    <row r="10" spans="2:7">
+      <c r="C10" s="3">
         <v>248134705</v>
       </c>
-      <c r="D5" s="3">
-        <f>C5/1000000000</f>
+      <c r="D10" s="11">
+        <f>C10/1000000000</f>
         <v>0.24813470500000001</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
-      <c r="C6" s="3">
+    <row r="11" spans="2:7">
+      <c r="C11" s="3">
         <v>240164775</v>
       </c>
-      <c r="D6" s="3">
-        <f t="shared" ref="D6:D10" si="0">C6/1000000000</f>
+      <c r="D11" s="11">
+        <f t="shared" ref="D11:D15" si="1">C11/1000000000</f>
         <v>0.240164775</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
-      <c r="C7" s="3">
+    <row r="12" spans="2:7">
+      <c r="C12" s="3">
         <v>231290725</v>
       </c>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
+      <c r="D12" s="11">
+        <f t="shared" si="1"/>
         <v>0.231290725</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
+    <row r="13" spans="2:7">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5">
         <v>244781156</v>
       </c>
-      <c r="D8" s="5">
-        <f t="shared" si="0"/>
+      <c r="D13" s="15">
+        <f t="shared" si="1"/>
         <v>0.244781156</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="2" t="s">
+    <row r="14" spans="2:7">
+      <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3">
-        <f>AVERAGE(C4:C8)</f>
-        <v>235389462.59999999</v>
-      </c>
-      <c r="D9" s="6">
-        <f t="shared" si="0"/>
-        <v>0.23538946259999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="2" t="s">
+      <c r="C14" s="12">
+        <f>AVERAGE(C4:C13)</f>
+        <v>222482209.90000001</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="1"/>
+        <v>0.22248220990000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3">
-        <f>C9/7776</f>
-        <v>30271.278626543208</v>
-      </c>
-      <c r="D10" s="6">
-        <f t="shared" si="0"/>
-        <v>3.0271278626543209E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="8" t="s">
+      <c r="C15" s="12">
+        <f>C14/7776</f>
+        <v>28611.39530606996</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>2.861139530606996E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="2">
-        <f>55^33</f>
-        <v>2.703763826271497E+57</v>
-      </c>
-      <c r="C13" s="3">
-        <f>B13*C10</f>
-        <v>8.1846388125433047E+61</v>
-      </c>
-      <c r="D13" s="3">
-        <f>D10*B13</f>
-        <v>8.1846388125433057E+52</v>
-      </c>
-      <c r="E13" s="2">
-        <f>D13/(60*60)</f>
-        <v>2.2735107812620294E+49</v>
-      </c>
-      <c r="F13" s="2">
-        <f>E13/24</f>
-        <v>9.4729615885917893E+47</v>
-      </c>
-      <c r="G13" s="2">
-        <f>F13/365</f>
-        <v>2.5953319420799422E+45</v>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="2">
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="C18" s="3">
+        <f>B18*C15</f>
+        <v>2.3594328972550347E+61</v>
+      </c>
+      <c r="D18" s="3">
+        <f>D15*B18</f>
+        <v>2.3594328972550347E+52</v>
+      </c>
+      <c r="E18" s="2">
+        <f>D18/(60*60)</f>
+        <v>6.5539802701528737E+48</v>
+      </c>
+      <c r="F18" s="2">
+        <f>E18/24</f>
+        <v>2.7308251125636974E+47</v>
+      </c>
+      <c r="G18" s="2">
+        <f>F18/365</f>
+        <v>7.4817126371608147E+44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -708,7 +793,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -740,17 +825,17 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="3">
         <v>22576583</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="11">
         <f>C4/1000000000</f>
         <v>2.2576583000000001E-2</v>
       </c>
@@ -759,7 +844,7 @@
       <c r="C5" s="3">
         <v>34172763</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="11">
         <f>C5/1000000000</f>
         <v>3.4172763000000002E-2</v>
       </c>
@@ -768,7 +853,7 @@
       <c r="C6" s="3">
         <v>18576956</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="11">
         <f t="shared" ref="D6:D10" si="0">C6/1000000000</f>
         <v>1.8576955999999999E-2</v>
       </c>
@@ -777,7 +862,7 @@
       <c r="C7" s="3">
         <v>16244818</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>1.6244818000000001E-2</v>
       </c>
@@ -787,7 +872,7 @@
       <c r="C8" s="5">
         <v>18095574</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="15">
         <f t="shared" si="0"/>
         <v>1.8095574E-2</v>
       </c>
@@ -796,11 +881,11 @@
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="12">
         <f>AVERAGE(C4:C8)</f>
         <v>21933338.800000001</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="16">
         <f t="shared" si="0"/>
         <v>2.19333388E-2</v>
       </c>
@@ -809,7 +894,7 @@
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="12">
         <f>C9/7776</f>
         <v>2820.6454218106996</v>
       </c>
@@ -819,10 +904,10 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:7">
@@ -869,16 +954,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -906,17 +990,17 @@
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="2:9">
       <c r="C4" s="3">
         <v>18724058</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="11">
         <f>C4/1000000000</f>
         <v>1.8724057999999998E-2</v>
       </c>
@@ -925,7 +1009,7 @@
       <c r="C5" s="3">
         <v>25851937</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="11">
         <f>C5/1000000000</f>
         <v>2.5851936999999998E-2</v>
       </c>
@@ -934,7 +1018,7 @@
       <c r="C6" s="3">
         <v>17988546</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="11">
         <f t="shared" ref="D6:D11" si="0">C6/1000000000</f>
         <v>1.7988546000000001E-2</v>
       </c>
@@ -943,7 +1027,7 @@
       <c r="C7" s="3">
         <v>19676560</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>1.9676559999999999E-2</v>
       </c>
@@ -953,7 +1037,7 @@
       <c r="C8" s="5">
         <v>15555244</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="15">
         <f t="shared" si="0"/>
         <v>1.5555243999999999E-2</v>
       </c>
@@ -966,7 +1050,7 @@
         <f>AVERAGE(C4:C8)</f>
         <v>19559269</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="16">
         <f t="shared" si="0"/>
         <v>1.9559269000000001E-2</v>
       </c>
@@ -975,11 +1059,11 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="12">
         <f>C9/7776</f>
         <v>2515.3380915637858</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="14">
         <f t="shared" si="0"/>
         <v>2.5153380915637856E-6</v>
       </c>
@@ -988,7 +1072,7 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="13">
         <f>C9/5346</f>
         <v>3658.6735877291435</v>
       </c>
@@ -998,58 +1082,58 @@
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="2">
-        <f>55^33</f>
-        <v>2.703763826271497E+57</v>
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
       </c>
       <c r="C14" s="3">
         <f>B14*C10</f>
-        <v>6.8008801428129461E+60</v>
+        <v>2.0742684435579487E+60</v>
       </c>
       <c r="D14" s="3">
         <f>D10*B14</f>
-        <v>6.8008801428129466E+51</v>
+        <v>2.0742684435579485E+51</v>
       </c>
       <c r="E14" s="2">
         <f>D14/(60*60)</f>
-        <v>1.8891333730035963E+48</v>
+        <v>5.7618567876609684E+47</v>
       </c>
       <c r="F14" s="2">
         <f>E14/24</f>
-        <v>7.8713890541816516E+46</v>
+        <v>2.4007736615254035E+46</v>
       </c>
       <c r="G14" s="2">
         <f>F14/365</f>
-        <v>2.1565449463511374E+44</v>
+        <v>6.5774620863709689E+43</v>
       </c>
     </row>
     <row r="15" spans="2:9">
       <c r="C15" s="3">
         <f>C11*B14</f>
-        <v>9.8921892986370147E+60</v>
+        <v>3.0171177360842891E+60</v>
       </c>
       <c r="D15" s="3">
         <f>D11*B14</f>
-        <v>9.8921892986370145E+51</v>
+        <v>3.0171177360842896E+51</v>
       </c>
       <c r="E15" s="2">
         <f>D15/(60*60)</f>
-        <v>2.7478303607325042E+48</v>
+        <v>8.3808826002341372E+47</v>
       </c>
       <c r="F15" s="2">
         <f>E15/24</f>
-        <v>1.1449293169718767E+47</v>
+        <v>3.4920344167642238E+46</v>
       </c>
       <c r="G15" s="2">
         <f>F15/365</f>
-        <v>3.1367926492380185E+44</v>
+        <v>9.5672175801759561E+43</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -1081,17 +1165,17 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="2:9">
       <c r="C21" s="3">
         <v>21177397</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="11">
         <f>C21/1000000000</f>
         <v>2.1177397000000001E-2</v>
       </c>
@@ -1100,7 +1184,7 @@
       <c r="C22" s="3">
         <v>9723433</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="11">
         <f>C22/1000000000</f>
         <v>9.7234330000000001E-3</v>
       </c>
@@ -1109,7 +1193,7 @@
       <c r="C23" s="3">
         <v>17796970</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="11">
         <f t="shared" ref="D23:D28" si="1">C23/1000000000</f>
         <v>1.7796969999999999E-2</v>
       </c>
@@ -1118,7 +1202,7 @@
       <c r="C24" s="3">
         <v>21073791</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="11">
         <f t="shared" si="1"/>
         <v>2.1073791000000001E-2</v>
       </c>
@@ -1128,7 +1212,7 @@
       <c r="C25" s="5">
         <v>18971347</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="15">
         <f t="shared" si="1"/>
         <v>1.8971347E-2</v>
       </c>
@@ -1137,11 +1221,11 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="12">
         <f>AVERAGE(C21:C25)</f>
         <v>17748587.600000001</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="16">
         <f t="shared" si="1"/>
         <v>1.7748587600000001E-2</v>
       </c>
@@ -1150,7 +1234,7 @@
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="12">
         <f>C26/7776</f>
         <v>2282.4829732510289</v>
       </c>
@@ -1163,7 +1247,7 @@
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="13">
         <f>C26/2376</f>
         <v>7469.9442760942766</v>
       </c>
@@ -1173,58 +1257,58 @@
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="2">
-        <f>55^33</f>
-        <v>2.703763826271497E+57</v>
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
       </c>
       <c r="C31" s="3">
         <f>B31*C27</f>
-        <v>6.1712948971567445E+60</v>
+        <v>1.8822449436328071E+60</v>
       </c>
       <c r="D31" s="3">
         <f>D27*B31</f>
-        <v>6.1712948971567455E+51</v>
+        <v>1.8822449436328071E+51</v>
       </c>
       <c r="E31" s="2">
         <f>D31/(60*60)</f>
-        <v>1.7142485825435405E+48</v>
+        <v>5.2284581767577971E+47</v>
       </c>
       <c r="F31" s="2">
         <f>E31/24</f>
-        <v>7.1427024272647519E+46</v>
+        <v>2.1785242403157487E+46</v>
       </c>
       <c r="G31" s="2">
         <f>F31/365</f>
-        <v>1.9569047745930828E+44</v>
+        <v>5.9685595625089008E+43</v>
       </c>
     </row>
     <row r="32" spans="2:9">
       <c r="C32" s="3">
         <f>C28*B31</f>
-        <v>2.0196965117967529E+61</v>
+        <v>6.1600743609800957E+60</v>
       </c>
       <c r="D32" s="3">
         <f>D28*B31</f>
-        <v>2.0196965117967531E+52</v>
+        <v>6.1600743609800961E+51</v>
       </c>
       <c r="E32" s="2">
         <f>D32/(60*60)</f>
-        <v>5.610268088324314E+48</v>
+        <v>1.7111317669389155E+48</v>
       </c>
       <c r="F32" s="2">
         <f>E32/24</f>
-        <v>2.3376117034684643E+47</v>
+        <v>7.1297156955788142E+46</v>
       </c>
       <c r="G32" s="2">
         <f>F32/365</f>
-        <v>6.4044156259409982E+44</v>
+        <v>1.9533467659120041E+44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toevoegen van schatting 5 kanalen, 9 comparators
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tester" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>Tester</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>zonder dubbels (1,2)(1,2)</t>
+  </si>
+  <si>
+    <t>5 channels, 9 comparators:</t>
   </si>
 </sst>
 </file>
@@ -76,8 +79,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="176" formatCode="0.00000E+00;\_x0000_"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000E+00;\_x0000_"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -119,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +138,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,7 +166,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -181,8 +190,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,27 +224,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="33">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -237,6 +258,11 @@
     <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -248,6 +274,11 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,18 +644,21 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="8"/>
+      <c r="B4" s="17">
+        <f>6^5</f>
+        <v>7776</v>
+      </c>
       <c r="C4" s="3">
         <v>207773446</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f>C4/1000000000</f>
         <v>0.207773446</v>
       </c>
@@ -634,7 +668,7 @@
       <c r="C5" s="3">
         <v>205065950</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f t="shared" ref="D5:D8" si="0">C5/1000000000</f>
         <v>0.20506595</v>
       </c>
@@ -644,7 +678,7 @@
       <c r="C6" s="3">
         <v>205841056</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f t="shared" si="0"/>
         <v>0.20584105599999999</v>
       </c>
@@ -654,7 +688,7 @@
       <c r="C7" s="3">
         <v>214539254</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>0.21453925400000001</v>
       </c>
@@ -664,7 +698,7 @@
       <c r="C8" s="3">
         <v>214655080</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f t="shared" si="0"/>
         <v>0.21465508</v>
       </c>
@@ -673,7 +707,7 @@
       <c r="C9" s="3">
         <v>212575952</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f>C9/1000000000</f>
         <v>0.21257595200000001</v>
       </c>
@@ -682,7 +716,7 @@
       <c r="C10" s="3">
         <v>248134705</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <f>C10/1000000000</f>
         <v>0.24813470500000001</v>
       </c>
@@ -691,7 +725,7 @@
       <c r="C11" s="3">
         <v>240164775</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <f t="shared" ref="D11:D15" si="1">C11/1000000000</f>
         <v>0.240164775</v>
       </c>
@@ -700,7 +734,7 @@
       <c r="C12" s="3">
         <v>231290725</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f t="shared" si="1"/>
         <v>0.231290725</v>
       </c>
@@ -710,7 +744,7 @@
       <c r="C13" s="5">
         <v>244781156</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <f t="shared" si="1"/>
         <v>0.244781156</v>
       </c>
@@ -719,11 +753,11 @@
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <f>AVERAGE(C4:C13)</f>
         <v>222482209.90000001</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="15">
         <f t="shared" si="1"/>
         <v>0.22248220990000001</v>
       </c>
@@ -732,7 +766,7 @@
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <f>C14/7776</f>
         <v>28611.39530606996</v>
       </c>
@@ -742,18 +776,18 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="2">
+      <c r="B18" s="17">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
       </c>
       <c r="C18" s="3">
-        <f>B18*C15</f>
+        <f>B18*$C$15</f>
         <v>2.3594328972550347E+61</v>
       </c>
       <c r="D18" s="3">
@@ -773,10 +807,47 @@
         <v>7.4817126371608147E+44</v>
       </c>
     </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="17">
+        <f>10^9  *0.305</f>
+        <v>305000000</v>
+      </c>
+      <c r="C21" s="3">
+        <f>B21*$C$15</f>
+        <v>8726475568351.3379</v>
+      </c>
+      <c r="D21" s="10">
+        <f>$D$15*B21</f>
+        <v>8726.4755683513376</v>
+      </c>
+      <c r="E21" s="18">
+        <f>D21/(60*60)</f>
+        <v>2.424020991208705</v>
+      </c>
+      <c r="F21" s="18">
+        <f>E21/24</f>
+        <v>0.10100087463369604</v>
+      </c>
+      <c r="G21" s="18">
+        <f>F21/365</f>
+        <v>2.7671472502382478E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="11"/>
+      <c r="E22" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -825,17 +896,17 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="3">
         <v>22576583</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f>C4/1000000000</f>
         <v>2.2576583000000001E-2</v>
       </c>
@@ -844,7 +915,7 @@
       <c r="C5" s="3">
         <v>34172763</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f>C5/1000000000</f>
         <v>3.4172763000000002E-2</v>
       </c>
@@ -853,7 +924,7 @@
       <c r="C6" s="3">
         <v>18576956</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f t="shared" ref="D6:D10" si="0">C6/1000000000</f>
         <v>1.8576955999999999E-2</v>
       </c>
@@ -862,7 +933,7 @@
       <c r="C7" s="3">
         <v>16244818</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>1.6244818000000001E-2</v>
       </c>
@@ -872,7 +943,7 @@
       <c r="C8" s="5">
         <v>18095574</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>1.8095574E-2</v>
       </c>
@@ -881,11 +952,11 @@
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <f>AVERAGE(C4:C8)</f>
         <v>21933338.800000001</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <f t="shared" si="0"/>
         <v>2.19333388E-2</v>
       </c>
@@ -894,7 +965,7 @@
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f>C9/7776</f>
         <v>2820.6454218106996</v>
       </c>
@@ -904,10 +975,10 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:7">
@@ -955,7 +1026,7 @@
   <dimension ref="B2:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -963,7 +1034,9 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -990,17 +1063,17 @@
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="2:9">
       <c r="C4" s="3">
         <v>18724058</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f>C4/1000000000</f>
         <v>1.8724057999999998E-2</v>
       </c>
@@ -1009,7 +1082,7 @@
       <c r="C5" s="3">
         <v>25851937</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f>C5/1000000000</f>
         <v>2.5851936999999998E-2</v>
       </c>
@@ -1018,7 +1091,7 @@
       <c r="C6" s="3">
         <v>17988546</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f t="shared" ref="D6:D11" si="0">C6/1000000000</f>
         <v>1.7988546000000001E-2</v>
       </c>
@@ -1027,7 +1100,7 @@
       <c r="C7" s="3">
         <v>19676560</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>1.9676559999999999E-2</v>
       </c>
@@ -1037,7 +1110,7 @@
       <c r="C8" s="5">
         <v>15555244</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>1.5555243999999999E-2</v>
       </c>
@@ -1050,7 +1123,7 @@
         <f>AVERAGE(C4:C8)</f>
         <v>19559269</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <f t="shared" si="0"/>
         <v>1.9559269000000001E-2</v>
       </c>
@@ -1059,11 +1132,11 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f>C9/7776</f>
         <v>2515.3380915637858</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <f t="shared" si="0"/>
         <v>2.5153380915637856E-6</v>
       </c>
@@ -1072,7 +1145,7 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <f>C9/5346</f>
         <v>3658.6735877291435</v>
       </c>
@@ -1082,10 +1155,10 @@
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:9">
@@ -1165,17 +1238,17 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="2:9">
       <c r="C21" s="3">
         <v>21177397</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="10">
         <f>C21/1000000000</f>
         <v>2.1177397000000001E-2</v>
       </c>
@@ -1184,7 +1257,7 @@
       <c r="C22" s="3">
         <v>9723433</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="10">
         <f>C22/1000000000</f>
         <v>9.7234330000000001E-3</v>
       </c>
@@ -1193,7 +1266,7 @@
       <c r="C23" s="3">
         <v>17796970</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <f t="shared" ref="D23:D28" si="1">C23/1000000000</f>
         <v>1.7796969999999999E-2</v>
       </c>
@@ -1202,7 +1275,7 @@
       <c r="C24" s="3">
         <v>21073791</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <f t="shared" si="1"/>
         <v>2.1073791000000001E-2</v>
       </c>
@@ -1212,7 +1285,7 @@
       <c r="C25" s="5">
         <v>18971347</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="14">
         <f t="shared" si="1"/>
         <v>1.8971347E-2</v>
       </c>
@@ -1221,11 +1294,11 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <f>AVERAGE(C21:C25)</f>
         <v>17748587.600000001</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <f t="shared" si="1"/>
         <v>1.7748587600000001E-2</v>
       </c>
@@ -1234,7 +1307,7 @@
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="11">
         <f>C26/7776</f>
         <v>2282.4829732510289</v>
       </c>
@@ -1247,7 +1320,7 @@
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="12">
         <f>C26/2376</f>
         <v>7469.9442760942766</v>
       </c>
@@ -1257,10 +1330,10 @@
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="2:9">

</xml_diff>

<commit_message>
Kleine veranderingen in lay-out
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tester" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Tester</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>5 channels, 9 comparators:</t>
+  </si>
+  <si>
+    <t>4 channels, 5 comparators: 2376 networks</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.00000E+00;\_x0000_"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +122,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -201,7 +210,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,11 +249,12 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -610,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -644,14 +654,14 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <f>6^5</f>
         <v>7776</v>
       </c>
@@ -776,13 +786,13 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="18"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
       </c>
@@ -808,13 +818,13 @@
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="18"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <f>10^9  *0.305</f>
         <v>305000000</v>
       </c>
@@ -826,15 +836,15 @@
         <f>$D$15*B21</f>
         <v>8726.4755683513376</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="17">
         <f>D21/(60*60)</f>
         <v>2.424020991208705</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <f>E21/24</f>
         <v>0.10100087463369604</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="17">
         <f>F21/365</f>
         <v>2.7671472502382478E-4</v>
       </c>
@@ -849,11 +859,12 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B20:C20"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
@@ -864,7 +875,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B2" sqref="B2:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -896,11 +907,11 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="3">
@@ -975,36 +986,36 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="2">
-        <f>55^33</f>
-        <v>2.703763826271497E+57</v>
+      <c r="B13" s="19">
+        <f>55^33 *0.305</f>
+        <v>8.2464796701280651E+56</v>
       </c>
       <c r="C13" s="3">
         <f>B13*C10</f>
-        <v>7.6263590582300777E+60</v>
+        <v>2.3260395127601736E+60</v>
       </c>
       <c r="D13" s="3">
         <f>D10*B13</f>
-        <v>7.626359058230078E+51</v>
+        <v>2.3260395127601736E+51</v>
       </c>
       <c r="E13" s="2">
         <f>D13/(60*60)</f>
-        <v>2.1184330717305773E+48</v>
+        <v>6.4612208687782603E+47</v>
       </c>
       <c r="F13" s="2">
         <f>E13/24</f>
-        <v>8.8268044655440716E+46</v>
+        <v>2.6921753619909419E+46</v>
       </c>
       <c r="G13" s="2">
         <f>F13/365</f>
-        <v>2.4183025932997458E+44</v>
+        <v>7.3758229095642241E+43</v>
       </c>
     </row>
   </sheetData>
@@ -1012,7 +1023,9 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B12:C12"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1025,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1034,7 +1047,7 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="2.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -1063,11 +1076,11 @@
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:9">
       <c r="C4" s="3">
@@ -1155,14 +1168,14 @@
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="2">
+      <c r="B14" s="19">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
       </c>
@@ -1213,7 +1226,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:9" s="9" customFormat="1"/>
+    <row r="17" spans="2:9" s="9" customFormat="1" ht="6" customHeight="1"/>
     <row r="19" spans="2:9">
       <c r="B19" s="1" t="s">
         <v>0</v>
@@ -1238,11 +1251,11 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
     </row>
     <row r="21" spans="2:9">
       <c r="C21" s="3">
@@ -1330,14 +1343,14 @@
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="2:9">
-      <c r="B31" s="2">
+      <c r="B31" s="19">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
       </c>
@@ -1391,11 +1404,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B30:C30"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Update tester zonder tijdsmeting van de I/O (bugfix)
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tester" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>Tester</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>4 channels, 5 comparators: 2376 networks</t>
+  </si>
+  <si>
+    <t>Aanpassing</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,8 +212,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,8 +260,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -273,6 +281,7 @@
     <cellStyle name="Gevolgde hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -289,6 +298,7 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G22"/>
+  <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -654,11 +664,11 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="16">
@@ -785,13 +795,13 @@
         <v>2.861139530606996E-5</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="18" t="s">
+    <row r="17" spans="1:7">
+      <c r="B17" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="2:7">
+      <c r="C17" s="20"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="B18" s="16">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
@@ -817,13 +827,13 @@
         <v>7.4817126371608147E+44</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="18" t="s">
+    <row r="20" spans="1:7">
+      <c r="B20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="18"/>
-    </row>
-    <row r="21" spans="2:7">
+      <c r="C20" s="20"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="B21" s="16">
         <f>10^9  *0.305</f>
         <v>305000000</v>
@@ -849,15 +859,243 @@
         <v>2.7671472502382478E-4</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="1:7">
       <c r="B22" s="11"/>
       <c r="E22" s="3"/>
     </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="16">
+        <f>6^5</f>
+        <v>7776</v>
+      </c>
+      <c r="C26" s="3">
+        <v>13034037</v>
+      </c>
+      <c r="D26" s="10">
+        <f>C26/1000000000</f>
+        <v>1.3034037E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="18"/>
+      <c r="C27" s="3">
+        <v>12317643</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" ref="D27:D30" si="2">C27/1000000000</f>
+        <v>1.2317643E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="18"/>
+      <c r="C28" s="3">
+        <v>13177732</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="2"/>
+        <v>1.3177731999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="18"/>
+      <c r="C29" s="3">
+        <v>12241814</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="2"/>
+        <v>1.2241814E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="18"/>
+      <c r="C30" s="3">
+        <v>12011124</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="2"/>
+        <v>1.2011124E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="C31" s="3">
+        <v>19439558</v>
+      </c>
+      <c r="D31" s="10">
+        <f>C31/1000000000</f>
+        <v>1.9439557999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="C32" s="3">
+        <v>18135757</v>
+      </c>
+      <c r="D32" s="10">
+        <f>C32/1000000000</f>
+        <v>1.8135756999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="C33" s="3">
+        <v>11970610</v>
+      </c>
+      <c r="D33" s="10">
+        <f t="shared" ref="D33:D37" si="3">C33/1000000000</f>
+        <v>1.197061E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="C34" s="3">
+        <v>10585078</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0585078E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5">
+        <v>14133194</v>
+      </c>
+      <c r="D35" s="14">
+        <f t="shared" si="3"/>
+        <v>1.4133194E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="11">
+        <f>AVERAGE(C26:C35)</f>
+        <v>13704654.699999999</v>
+      </c>
+      <c r="D36" s="15">
+        <f t="shared" si="3"/>
+        <v>1.3704654699999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="11">
+        <f>C36/7776</f>
+        <v>1762.4298739711933</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" si="3"/>
+        <v>1.7624298739711933E-6</v>
+      </c>
+      <c r="H37" s="2">
+        <f>C15/C37</f>
+        <v>16.23406169438184</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="20"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="16">
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="C40" s="3">
+        <f>B40*$C$37</f>
+        <v>1.4533842125729813E+60</v>
+      </c>
+      <c r="D40" s="3">
+        <f>D37*B40</f>
+        <v>1.4533842125729814E+51</v>
+      </c>
+      <c r="E40" s="2">
+        <f>D40/(60*60)</f>
+        <v>4.0371783682582814E+47</v>
+      </c>
+      <c r="F40" s="2">
+        <f>E40/24</f>
+        <v>1.6821576534409507E+46</v>
+      </c>
+      <c r="G40" s="2">
+        <f>F40/365</f>
+        <v>4.6086511053176733E+43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="20"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="16">
+        <f>10^9  *0.305</f>
+        <v>305000000</v>
+      </c>
+      <c r="C43" s="3">
+        <f>B43*$C$37</f>
+        <v>537541111561.21393</v>
+      </c>
+      <c r="D43" s="10">
+        <f>$D$37*B43</f>
+        <v>537.54111156121394</v>
+      </c>
+      <c r="E43" s="17">
+        <f>D43/(60*60)</f>
+        <v>0.14931697543367053</v>
+      </c>
+      <c r="F43" s="17">
+        <f>E43/24</f>
+        <v>6.2215406430696056E-3</v>
+      </c>
+      <c r="G43" s="17">
+        <f>F43/365</f>
+        <v>1.7045316830327687E-5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B39:C39"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -907,11 +1145,11 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:7">
       <c r="C4" s="3">
@@ -986,10 +1224,10 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:7">
@@ -1038,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1076,11 +1314,11 @@
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:9">
       <c r="C4" s="3">
@@ -1168,10 +1406,10 @@
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:9">
@@ -1251,11 +1489,11 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" spans="2:9">
       <c r="C21" s="3">
@@ -1343,10 +1581,10 @@
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="2:9">

</xml_diff>

<commit_message>
Nieuwe tijdsmetingen voor de derde generator.
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tester" sheetId="1" r:id="rId1"/>
     <sheet name="Generator1" sheetId="2" r:id="rId2"/>
     <sheet name="Generator2" sheetId="3" r:id="rId3"/>
+    <sheet name="Generator3" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
   <si>
     <t>Tester</t>
   </si>
@@ -630,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
@@ -1113,7 +1114,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1276,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1651,4 +1652,161 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="C4" s="3">
+        <v>703752522</v>
+      </c>
+      <c r="D4" s="10">
+        <f>C4/1000000000</f>
+        <v>0.70375252200000005</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="C5" s="3">
+        <v>683700922</v>
+      </c>
+      <c r="D5" s="10">
+        <f>C5/1000000000</f>
+        <v>0.68370092199999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="C6" s="3"/>
+      <c r="D6" s="10">
+        <f t="shared" ref="D6:D10" si="0">C6/1000000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="C7" s="3"/>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="11">
+        <f>AVERAGE(C4:C8)</f>
+        <v>693726722</v>
+      </c>
+      <c r="D9" s="15">
+        <f t="shared" si="0"/>
+        <v>0.69372672199999996</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11">
+        <f>C9/7776</f>
+        <v>89213.827417695473</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>8.9213827417695477E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="19">
+        <f>55^33 *0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="C13" s="3">
+        <f>B13*C10</f>
+        <v>7.3570001409433946E+61</v>
+      </c>
+      <c r="D13" s="3">
+        <f>D10*B13</f>
+        <v>7.357000140943395E+52</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13/(60*60)</f>
+        <v>2.0436111502620541E+49</v>
+      </c>
+      <c r="F13" s="2">
+        <f>E13/24</f>
+        <v>8.515046459425225E+47</v>
+      </c>
+      <c r="G13" s="2">
+        <f>F13/365</f>
+        <v>2.3328894409384179E+45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Toevoegen van resultaten voor de tijdsmetingen van - Generator 3 - Generator 4 - Tester 2
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tester" sheetId="1" r:id="rId1"/>
-    <sheet name="Generator1" sheetId="2" r:id="rId2"/>
-    <sheet name="Generator2" sheetId="3" r:id="rId3"/>
-    <sheet name="Generator3" sheetId="5" r:id="rId4"/>
+    <sheet name="Tester1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tester2" sheetId="7" r:id="rId2"/>
+    <sheet name="Generator1" sheetId="2" r:id="rId3"/>
+    <sheet name="Generator2" sheetId="3" r:id="rId4"/>
+    <sheet name="Generator3" sheetId="5" r:id="rId5"/>
+    <sheet name="Generator4" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
   <si>
     <t>Tester</t>
   </si>
@@ -79,6 +86,12 @@
   </si>
   <si>
     <t>Aanpassing</t>
+  </si>
+  <si>
+    <t>algorithme 1</t>
+  </si>
+  <si>
+    <t>algorithme 2</t>
   </si>
 </sst>
 </file>
@@ -216,7 +229,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,6 +277,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -300,10 +316,15 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -631,11 +652,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -644,7 +665,7 @@
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="1" customFormat="1">
+    <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,14 +685,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="16">
         <f>6^5</f>
         <v>7776</v>
@@ -684,7 +705,7 @@
         <v>0.207773446</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="8"/>
       <c r="C5" s="3">
         <v>205065950</v>
@@ -694,7 +715,7 @@
         <v>0.20506595</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="3">
         <v>205841056</v>
@@ -704,7 +725,7 @@
         <v>0.20584105599999999</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="3">
         <v>214539254</v>
@@ -714,7 +735,7 @@
         <v>0.21453925400000001</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
       <c r="C8" s="3">
         <v>214655080</v>
@@ -724,7 +745,7 @@
         <v>0.21465508</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
         <v>212575952</v>
       </c>
@@ -733,7 +754,7 @@
         <v>0.21257595200000001</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
         <v>248134705</v>
       </c>
@@ -742,7 +763,7 @@
         <v>0.24813470500000001</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
         <v>240164775</v>
       </c>
@@ -751,7 +772,7 @@
         <v>0.240164775</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C12" s="3">
         <v>231290725</v>
       </c>
@@ -760,7 +781,7 @@
         <v>0.231290725</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="5">
         <v>244781156</v>
@@ -770,7 +791,7 @@
         <v>0.244781156</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
@@ -783,7 +804,7 @@
         <v>0.22248220990000001</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
@@ -796,13 +817,13 @@
         <v>2.861139530606996E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="20"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="C17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="16">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
@@ -828,13 +849,13 @@
         <v>7.4817126371608147E+44</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="B20" s="20" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="20"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="C20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="16">
         <f>10^9  *0.305</f>
         <v>305000000</v>
@@ -860,16 +881,16 @@
         <v>2.7671472502382478E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,14 +910,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="B25" s="20" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="16">
         <f>6^5</f>
         <v>7776</v>
@@ -909,7 +930,7 @@
         <v>1.3034037E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="18"/>
       <c r="C27" s="3">
         <v>12317643</v>
@@ -919,7 +940,7 @@
         <v>1.2317643E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
       <c r="C28" s="3">
         <v>13177732</v>
@@ -929,7 +950,7 @@
         <v>1.3177731999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="18"/>
       <c r="C29" s="3">
         <v>12241814</v>
@@ -939,7 +960,7 @@
         <v>1.2241814E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="18"/>
       <c r="C30" s="3">
         <v>12011124</v>
@@ -949,7 +970,7 @@
         <v>1.2011124E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C31" s="3">
         <v>19439558</v>
       </c>
@@ -958,7 +979,7 @@
         <v>1.9439557999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
         <v>18135757</v>
       </c>
@@ -967,7 +988,7 @@
         <v>1.8135756999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C33" s="3">
         <v>11970610</v>
       </c>
@@ -976,7 +997,7 @@
         <v>1.197061E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>10585078</v>
       </c>
@@ -985,7 +1006,7 @@
         <v>1.0585078E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="5">
         <v>14133194</v>
@@ -995,7 +1016,7 @@
         <v>1.4133194E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +1029,7 @@
         <v>1.3704654699999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
@@ -1025,13 +1046,13 @@
         <v>16.23406169438184</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="20" t="s">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="20"/>
-    </row>
-    <row r="40" spans="2:8">
+      <c r="C39" s="21"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="16">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
@@ -1057,13 +1078,13 @@
         <v>4.6086511053176733E+43</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
-      <c r="B42" s="20" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="20"/>
-    </row>
-    <row r="43" spans="2:8">
+      <c r="C42" s="21"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" s="16">
         <f>10^9  *0.305</f>
         <v>305000000</v>
@@ -1101,15 +1122,695 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <f>6^5</f>
+        <v>7776</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6326955</v>
+      </c>
+      <c r="C4" s="10">
+        <f>B4/1000000000</f>
+        <v>6.3269550000000004E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="20"/>
+      <c r="B5" s="3">
+        <v>7374696</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" ref="C5:C8" si="0">B5/1000000000</f>
+        <v>7.374696E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="3">
+        <v>4570509</v>
+      </c>
+      <c r="C6" s="10">
+        <f t="shared" si="0"/>
+        <v>4.5705090000000004E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="3">
+        <v>4627635</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" si="0"/>
+        <v>4.6276349999999997E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="3">
+        <v>7627910</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" si="0"/>
+        <v>7.6279099999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
+        <v>7977839</v>
+      </c>
+      <c r="C9" s="10">
+        <f>B9/1000000000</f>
+        <v>7.9778390000000005E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <v>7907929</v>
+      </c>
+      <c r="C10" s="10">
+        <f>B10/1000000000</f>
+        <v>7.9079289999999993E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <v>4005073</v>
+      </c>
+      <c r="C11" s="10">
+        <f t="shared" ref="C11:C15" si="1">B11/1000000000</f>
+        <v>4.0050729999999996E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>6534141</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="1"/>
+        <v>6.5341410000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5">
+        <v>7755012</v>
+      </c>
+      <c r="C13" s="14">
+        <f t="shared" si="1"/>
+        <v>7.7550120000000004E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="11">
+        <f>AVERAGE(B4:B13)</f>
+        <v>6470769.9000000004</v>
+      </c>
+      <c r="C14" s="15">
+        <f t="shared" si="1"/>
+        <v>6.4707699000000002E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11">
+        <f>B14/A4</f>
+        <v>832.14633487654328</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>8.3214633487654324E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="16">
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="B18" s="3">
+        <f>A18*$B$15</f>
+        <v>6.8622778331309948E+59</v>
+      </c>
+      <c r="C18" s="3">
+        <f>C15*A18</f>
+        <v>6.8622778331309945E+50</v>
+      </c>
+      <c r="D18" s="2">
+        <f>C18/(60*60)</f>
+        <v>1.9061882869808318E+47</v>
+      </c>
+      <c r="E18" s="2">
+        <f>D18/24</f>
+        <v>7.9424511957534662E+45</v>
+      </c>
+      <c r="F18" s="2">
+        <f>E18/365</f>
+        <v>2.1760140262338263E+43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <f>10^9  *0.305</f>
+        <v>305000000</v>
+      </c>
+      <c r="B21" s="3">
+        <f>A21*$B$15</f>
+        <v>253804632137.3457</v>
+      </c>
+      <c r="C21" s="10">
+        <f>$C$15*A21</f>
+        <v>253.80463213734569</v>
+      </c>
+      <c r="D21" s="17">
+        <f>C21/(60*60)</f>
+        <v>7.0501286704818242E-2</v>
+      </c>
+      <c r="E21" s="17">
+        <f>D21/24</f>
+        <v>2.9375536127007602E-3</v>
+      </c>
+      <c r="F21" s="17">
+        <f>E21/365</f>
+        <v>8.0480920895911236E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
+        <f>6^5</f>
+        <v>7776</v>
+      </c>
+      <c r="B26" s="3">
+        <v>4254277</v>
+      </c>
+      <c r="C26" s="10">
+        <f>B26/1000000000</f>
+        <v>4.2542769999999999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="3">
+        <v>6781921</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" ref="C27:C30" si="2">B27/1000000000</f>
+        <v>6.7819209999999998E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="20"/>
+      <c r="B28" s="3">
+        <v>7915738</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="2"/>
+        <v>7.9157380000000003E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="3">
+        <v>7039516</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="2"/>
+        <v>7.039516E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="20"/>
+      <c r="B30" s="3">
+        <v>5099304</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="2"/>
+        <v>5.0993039999999998E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="3">
+        <v>4638402</v>
+      </c>
+      <c r="C31" s="10">
+        <f>B31/1000000000</f>
+        <v>4.6384019999999998E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="3">
+        <v>3917580</v>
+      </c>
+      <c r="C32" s="10">
+        <f>B32/1000000000</f>
+        <v>3.9175800000000004E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="3">
+        <v>5557205</v>
+      </c>
+      <c r="C33" s="10">
+        <f t="shared" ref="C33:C37" si="3">B33/1000000000</f>
+        <v>5.557205E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="3">
+        <v>9128796</v>
+      </c>
+      <c r="C34" s="10">
+        <f t="shared" si="3"/>
+        <v>9.1287959999999998E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5">
+        <v>5483936</v>
+      </c>
+      <c r="C35" s="14">
+        <f t="shared" si="3"/>
+        <v>5.483936E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="11">
+        <f>AVERAGE(B26:B35)</f>
+        <v>5981667.5</v>
+      </c>
+      <c r="C36" s="15">
+        <f t="shared" si="3"/>
+        <v>5.9816675000000001E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="11">
+        <f>B36/A26</f>
+        <v>769.24736368312756</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="3"/>
+        <v>7.6924736368312757E-7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="21"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="16">
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="B40" s="3">
+        <f>A40*$B$37</f>
+        <v>6.3435827459125214E+59</v>
+      </c>
+      <c r="C40" s="3">
+        <f>C37*A40</f>
+        <v>6.3435827459125214E+50</v>
+      </c>
+      <c r="D40" s="2">
+        <f>C40/(60*60)</f>
+        <v>1.7621063183090336E+47</v>
+      </c>
+      <c r="E40" s="2">
+        <f>D40/24</f>
+        <v>7.3421096596209735E+45</v>
+      </c>
+      <c r="F40" s="2">
+        <f>E40/365</f>
+        <v>2.011536893046842E+43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="16">
+        <f>10^9  *0.305</f>
+        <v>305000000</v>
+      </c>
+      <c r="B43" s="3">
+        <f>A43*$B$37</f>
+        <v>234620445923.35391</v>
+      </c>
+      <c r="C43" s="10">
+        <f>$C$37*A43</f>
+        <v>234.62044592335391</v>
+      </c>
+      <c r="D43" s="17">
+        <f>C43/(60*60)</f>
+        <v>6.5172346089820532E-2</v>
+      </c>
+      <c r="E43" s="17">
+        <f>D43/24</f>
+        <v>2.7155144204091888E-3</v>
+      </c>
+      <c r="F43" s="17">
+        <f>E43/365</f>
+        <v>7.4397655353676406E-6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="16">
+        <f>6^5</f>
+        <v>7776</v>
+      </c>
+      <c r="B48" s="3">
+        <v>6453530</v>
+      </c>
+      <c r="C48" s="10">
+        <f>B48/1000000000</f>
+        <v>6.4535299999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="3">
+        <v>3655165</v>
+      </c>
+      <c r="C49" s="10">
+        <f t="shared" ref="C49:C52" si="4">B49/1000000000</f>
+        <v>3.6551650000000002E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="3">
+        <v>8965547</v>
+      </c>
+      <c r="C50" s="10">
+        <f t="shared" si="4"/>
+        <v>8.9655470000000008E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="20"/>
+      <c r="B51" s="3">
+        <v>5729721</v>
+      </c>
+      <c r="C51" s="10">
+        <f t="shared" si="4"/>
+        <v>5.7297210000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="3">
+        <v>6674915</v>
+      </c>
+      <c r="C52" s="10">
+        <f t="shared" si="4"/>
+        <v>6.674915E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" s="3">
+        <v>4328111</v>
+      </c>
+      <c r="C53" s="10">
+        <f>B53/1000000000</f>
+        <v>4.3281109999999999E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" s="3">
+        <v>3770450</v>
+      </c>
+      <c r="C54" s="10">
+        <f>B54/1000000000</f>
+        <v>3.7704499999999998E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" s="3">
+        <v>4608586</v>
+      </c>
+      <c r="C55" s="10">
+        <f t="shared" ref="C55:C59" si="5">B55/1000000000</f>
+        <v>4.6085859999999996E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56" s="3">
+        <v>4937503</v>
+      </c>
+      <c r="C56" s="10">
+        <f t="shared" si="5"/>
+        <v>4.9375030000000002E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5">
+        <v>6335713</v>
+      </c>
+      <c r="C57" s="14">
+        <f t="shared" si="5"/>
+        <v>6.3357129999999998E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="11">
+        <f>AVERAGE(B48:B57)</f>
+        <v>5545924.0999999996</v>
+      </c>
+      <c r="C58" s="15">
+        <f t="shared" si="5"/>
+        <v>5.5459240999999994E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="11">
+        <f>B58/A48</f>
+        <v>713.21040380658428</v>
+      </c>
+      <c r="C59" s="6">
+        <f t="shared" si="5"/>
+        <v>7.1321040380658432E-7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="21"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="16">
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="B62" s="3">
+        <f>A62*$B$59</f>
+        <v>5.8814750955148251E+59</v>
+      </c>
+      <c r="C62" s="3">
+        <f>C59*A62</f>
+        <v>5.8814750955148256E+50</v>
+      </c>
+      <c r="D62" s="2">
+        <f>C62/(60*60)</f>
+        <v>1.6337430820874515E+47</v>
+      </c>
+      <c r="E62" s="2">
+        <f>D62/24</f>
+        <v>6.807262842031048E+45</v>
+      </c>
+      <c r="F62" s="2">
+        <f>E62/365</f>
+        <v>1.8650035183646706E+43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="21"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="16">
+        <f>10^9  *0.305</f>
+        <v>305000000</v>
+      </c>
+      <c r="B65" s="3">
+        <f>A65*$B$59</f>
+        <v>217529173161.00821</v>
+      </c>
+      <c r="C65" s="10">
+        <f>$C$59*A65</f>
+        <v>217.5291731610082</v>
+      </c>
+      <c r="D65" s="17">
+        <f>C65/(60*60)</f>
+        <v>6.0424770322502278E-2</v>
+      </c>
+      <c r="E65" s="17">
+        <f>D65/24</f>
+        <v>2.5176987634375949E-3</v>
+      </c>
+      <c r="F65" s="17">
+        <f>E65/365</f>
+        <v>6.8978048313358762E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A42:B42"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G13"/>
   <sheetViews>
@@ -1117,7 +1818,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -1125,7 +1826,7 @@
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,14 +1846,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>22576583</v>
       </c>
@@ -1161,7 +1862,7 @@
         <v>2.2576583000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>34172763</v>
       </c>
@@ -1170,7 +1871,7 @@
         <v>3.4172763000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <v>18576956</v>
       </c>
@@ -1179,7 +1880,7 @@
         <v>1.8576955999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
         <v>16244818</v>
       </c>
@@ -1188,7 +1889,7 @@
         <v>1.6244818000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="5">
         <v>18095574</v>
@@ -1198,7 +1899,7 @@
         <v>1.8095574E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1211,7 +1912,7 @@
         <v>2.19333388E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1224,14 +1925,14 @@
         <v>2.8206454218106995E-6</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="20" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="19">
         <f>55^33 *0.305</f>
         <v>8.2464796701280651E+56</v>
@@ -1265,23 +1966,18 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -1291,7 +1987,7 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,14 +2010,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="2:9">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>18724058</v>
       </c>
@@ -1330,7 +2026,7 @@
         <v>1.8724057999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>25851937</v>
       </c>
@@ -1339,7 +2035,7 @@
         <v>2.5851936999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <v>17988546</v>
       </c>
@@ -1348,7 +2044,7 @@
         <v>1.7988546000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
         <v>19676560</v>
       </c>
@@ -1357,7 +2053,7 @@
         <v>1.9676559999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="5">
         <v>15555244</v>
@@ -1367,7 +2063,7 @@
         <v>1.5555243999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1380,7 +2076,7 @@
         <v>1.9559269000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1393,7 +2089,7 @@
         <v>2.5153380915637856E-6</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1406,14 +2102,14 @@
         <v>3.6586735877291436E-6</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="19">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
@@ -1439,7 +2135,7 @@
         <v>6.5774620863709689E+43</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
         <f>C11*B14</f>
         <v>3.0171177360842891E+60</v>
@@ -1461,12 +2157,12 @@
         <v>9.5672175801759561E+43</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:9" s="9" customFormat="1" ht="6" customHeight="1"/>
-    <row r="19" spans="2:9">
+    <row r="17" spans="2:9" s="9" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1489,14 +2185,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
-      <c r="B20" s="20" t="s">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C21" s="3">
         <v>21177397</v>
       </c>
@@ -1505,7 +2201,7 @@
         <v>2.1177397000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
         <v>9723433</v>
       </c>
@@ -1514,7 +2210,7 @@
         <v>9.7234330000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
         <v>17796970</v>
       </c>
@@ -1523,7 +2219,7 @@
         <v>1.7796969999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C24" s="3">
         <v>21073791</v>
       </c>
@@ -1532,7 +2228,7 @@
         <v>2.1073791000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
       <c r="C25" s="5">
         <v>18971347</v>
@@ -1542,7 +2238,7 @@
         <v>1.8971347E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
@@ -1555,7 +2251,7 @@
         <v>1.7748587600000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
@@ -1568,7 +2264,7 @@
         <v>2.2824829732510289E-6</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1581,14 +2277,14 @@
         <v>7.4699442760942768E-6</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
-      <c r="B30" s="20" t="s">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="19">
         <f>(55^33)*0.305</f>
         <v>8.2464796701280651E+56</v>
@@ -1614,7 +2310,7 @@
         <v>5.9685595625089008E+43</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C32" s="3">
         <f>C28*B31</f>
         <v>6.1600743609800957E+60</v>
@@ -1646,23 +2342,18 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G13"/>
+  <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -1670,7 +2361,7 @@
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1689,124 +2380,575 @@
       <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="20" t="s">
+      <c r="I2" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="20"/>
       <c r="C4" s="3">
-        <v>703752522</v>
+        <v>529770</v>
       </c>
       <c r="D4" s="10">
-        <f>C4/1000000000</f>
-        <v>0.70375252200000005</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
+        <f t="shared" ref="D4:D8" si="0">C4/1000000000</f>
+        <v>5.2977000000000005E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="20"/>
       <c r="C5" s="3">
-        <v>683700922</v>
+        <v>685671</v>
       </c>
       <c r="D5" s="10">
-        <f>C5/1000000000</f>
-        <v>0.68370092199999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="C6" s="3"/>
+        <f t="shared" si="0"/>
+        <v>6.85671E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="20"/>
+      <c r="C6" s="3">
+        <v>509244</v>
+      </c>
       <c r="D6" s="10">
-        <f t="shared" ref="D6:D10" si="0">C6/1000000000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="C7" s="3"/>
+        <f t="shared" si="0"/>
+        <v>5.0924399999999995E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="20"/>
+      <c r="C7" s="3">
+        <v>781948</v>
+      </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
+        <v>7.8194799999999997E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="20"/>
+      <c r="C8" s="3">
+        <v>681762</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>6.8176200000000004E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>466237</v>
+      </c>
+      <c r="D9" s="10">
+        <f>C9/1000000000</f>
+        <v>4.6623699999999999E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
+        <v>1870811</v>
+      </c>
+      <c r="D10" s="10">
+        <f>C10/1000000000</f>
+        <v>1.870811E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <v>461350</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" ref="D11:D15" si="1">C11/1000000000</f>
+        <v>4.6135000000000002E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="3">
+        <v>806873</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="1"/>
+        <v>8.0687300000000005E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5">
+        <v>568867</v>
+      </c>
+      <c r="D13" s="14">
+        <f t="shared" si="1"/>
+        <v>5.6886700000000003E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="11">
+        <f>AVERAGE(C4:C13)</f>
+        <v>736253.3</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="1"/>
+        <v>7.3625330000000007E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="11">
+        <f>C14/7776</f>
+        <v>94.682780349794243</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>9.4682780349794244E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="19">
+        <f>(55^33) *0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="C18" s="3">
+        <f>B18*C15</f>
+        <v>7.8079962326577926E+58</v>
+      </c>
+      <c r="D18" s="3">
+        <f>D15*B18</f>
+        <v>7.8079962326577928E+49</v>
+      </c>
+      <c r="E18" s="2">
+        <f>D18/(60*60)</f>
+        <v>2.1688878424049423E+46</v>
+      </c>
+      <c r="F18" s="2">
+        <f>E18/24</f>
+        <v>9.0370326766872597E+44</v>
+      </c>
+      <c r="G18" s="2">
+        <f>F18/365</f>
+        <v>2.4758993634759615E+42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="2" t="s">
+      <c r="C21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="20"/>
+      <c r="C23" s="3">
+        <v>540033</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" ref="D23:D27" si="2">C23/1000000000</f>
+        <v>5.4003299999999998E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="20"/>
+      <c r="C24" s="3">
+        <v>478455</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="2"/>
+        <v>4.7845500000000003E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="20"/>
+      <c r="C25" s="3">
+        <v>825933</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" si="2"/>
+        <v>8.2593300000000005E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="20"/>
+      <c r="C26" s="3">
+        <v>457440</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="2"/>
+        <v>4.5743999999999998E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="20"/>
+      <c r="C27" s="3">
+        <v>458906</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="2"/>
+        <v>4.5890599999999997E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="3">
+        <v>525372</v>
+      </c>
+      <c r="D28" s="10">
+        <f>C28/1000000000</f>
+        <v>5.2537199999999997E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="3">
+        <v>506312</v>
+      </c>
+      <c r="D29" s="10">
+        <f>C29/1000000000</f>
+        <v>5.0631199999999997E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="3">
+        <v>795144</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" ref="D30:D34" si="3">C30/1000000000</f>
+        <v>7.9514400000000002E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C31" s="3">
+        <v>1086908</v>
+      </c>
+      <c r="D31" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0869079999999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="5">
+        <v>507289</v>
+      </c>
+      <c r="D32" s="14">
+        <f t="shared" si="3"/>
+        <v>5.0728899999999996E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="11">
-        <f>AVERAGE(C4:C8)</f>
-        <v>693726722</v>
-      </c>
-      <c r="D9" s="15">
-        <f t="shared" si="0"/>
-        <v>0.69372672199999996</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="2" t="s">
+      <c r="C33" s="11">
+        <f>AVERAGE(C23:C32)</f>
+        <v>618179.19999999995</v>
+      </c>
+      <c r="D33" s="15">
+        <f t="shared" si="3"/>
+        <v>6.1817919999999991E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="11">
-        <f>C9/7776</f>
-        <v>89213.827417695473</v>
-      </c>
-      <c r="D10" s="6">
-        <f t="shared" si="0"/>
-        <v>8.9213827417695477E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="20" t="s">
+      <c r="C34" s="11">
+        <f>C33/7776</f>
+        <v>79.49835390946501</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="3"/>
+        <v>7.9498353909465004E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="19">
-        <f>55^33 *0.305</f>
+      <c r="C36" s="21"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="19">
+        <f>(55^33) *0.305</f>
         <v>8.2464796701280651E+56</v>
       </c>
-      <c r="C13" s="3">
-        <f>B13*C10</f>
-        <v>7.3570001409433946E+61</v>
-      </c>
-      <c r="D13" s="3">
-        <f>D10*B13</f>
-        <v>7.357000140943395E+52</v>
-      </c>
-      <c r="E13" s="2">
-        <f>D13/(60*60)</f>
-        <v>2.0436111502620541E+49</v>
-      </c>
-      <c r="F13" s="2">
-        <f>E13/24</f>
-        <v>8.515046459425225E+47</v>
-      </c>
-      <c r="G13" s="2">
-        <f>F13/365</f>
-        <v>2.3328894409384179E+45</v>
+      <c r="C37" s="3">
+        <f>B37*C34</f>
+        <v>6.555815593230492E+58</v>
+      </c>
+      <c r="D37" s="3">
+        <f>D34*B37</f>
+        <v>6.5558155932304914E+49</v>
+      </c>
+      <c r="E37" s="2">
+        <f>D37/(60*60)</f>
+        <v>1.8210598870084698E+46</v>
+      </c>
+      <c r="F37" s="2">
+        <f>E37/24</f>
+        <v>7.5877495292019577E+44</v>
+      </c>
+      <c r="G37" s="2">
+        <f>F37/365</f>
+        <v>2.0788354874525911E+42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="20"/>
+      <c r="C3" s="3">
+        <v>526349</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" ref="D3:D7" si="0">C3/1000000000</f>
+        <v>5.2634899999999996E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="20"/>
+      <c r="C4" s="3">
+        <v>685671</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>6.85671E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="20"/>
+      <c r="C5" s="3">
+        <v>684205</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>6.8420500000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="20"/>
+      <c r="C6" s="3">
+        <v>582063</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>5.8206299999999996E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="20"/>
+      <c r="C7" s="3">
+        <v>689581</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>6.8958099999999998E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
+        <v>1400176</v>
+      </c>
+      <c r="D8" s="10">
+        <f>C8/1000000000</f>
+        <v>1.4001759999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>1008713</v>
+      </c>
+      <c r="D9" s="10">
+        <f>C9/1000000000</f>
+        <v>1.0087130000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
+        <v>639243</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" ref="D10:D14" si="1">C10/1000000000</f>
+        <v>6.3924299999999995E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <v>661724</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>6.6172400000000004E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5">
+        <v>628980</v>
+      </c>
+      <c r="D12" s="14">
+        <f t="shared" si="1"/>
+        <v>6.2898000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="11">
+        <f>AVERAGE(C3:C12)</f>
+        <v>750670.5</v>
+      </c>
+      <c r="D13" s="15">
+        <f t="shared" si="1"/>
+        <v>7.506705E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="12">
+        <f>C13/2376</f>
+        <v>315.93876262626264</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1593876262626267E-7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="19">
+        <f>(55^33)*0.305</f>
+        <v>8.2464796701280651E+56</v>
+      </c>
+      <c r="C17" s="3">
+        <f>C14*B17</f>
+        <v>2.6053825830028913E+59</v>
+      </c>
+      <c r="D17" s="3">
+        <f>D14*B17</f>
+        <v>2.6053825830028916E+50</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17/(60*60)</f>
+        <v>7.2371738416746987E+46</v>
+      </c>
+      <c r="F17" s="2">
+        <f>E17/24</f>
+        <v>3.0154891006977913E+45</v>
+      </c>
+      <c r="G17" s="2">
+        <f>F17/365</f>
+        <v>8.2616139745144972E+42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B16:C16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Toevoegen van samenvattend tabblad timeTest
</commit_message>
<xml_diff>
--- a/timeTest.xlsx
+++ b/timeTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Tester1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Generator2" sheetId="3" r:id="rId4"/>
     <sheet name="Generator3" sheetId="5" r:id="rId5"/>
     <sheet name="Generator4" sheetId="6" r:id="rId6"/>
+    <sheet name="Samenvatting" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
   <si>
     <t>Tester</t>
   </si>
@@ -93,16 +94,46 @@
   <si>
     <t>algorithme 2</t>
   </si>
+  <si>
+    <t>Tester 1</t>
+  </si>
+  <si>
+    <t>1 netwerk [ns]</t>
+  </si>
+  <si>
+    <t>Tester 2</t>
+  </si>
+  <si>
+    <t>Generator 1</t>
+  </si>
+  <si>
+    <t>Generator 2</t>
+  </si>
+  <si>
+    <t>Generator 3</t>
+  </si>
+  <si>
+    <t>Generator 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.00000E+00;\_x0000_"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +174,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,44 +230,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,10 +285,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -268,20 +308,25 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -316,6 +361,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Komma" xfId="35" builtinId="3"/>
+    <cellStyle name="Procent" xfId="36" builtinId="5"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A15" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -1119,7 +1166,7 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B39:C39"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -1129,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F65"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A35" zoomScale="94" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A38" zoomScale="94" workbookViewId="0">
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
@@ -1963,7 +2010,7 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B12:C12"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -1973,7 +2020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2339,7 +2386,7 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B30:C30"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -2349,7 +2396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A8" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -2747,7 +2794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2951,4 +2998,99 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="23">
+        <f>Tester1!C37</f>
+        <v>1762.4298739711933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="23">
+        <f>Tester2!B59</f>
+        <v>713.21040380658428</v>
+      </c>
+      <c r="C3" s="24">
+        <f>ABS(B2-B3)/B2</f>
+        <v>0.59532551374680021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="23">
+        <f>Generator1!C10</f>
+        <v>2820.6454218106996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="23">
+        <f>Generator3!C34</f>
+        <v>79.49835390946501</v>
+      </c>
+      <c r="C6" s="24">
+        <f>ABS(B5-B6)/B5</f>
+        <v>0.97181554501861789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="23">
+        <f>Generator2!C28</f>
+        <v>7469.9442760942766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="23">
+        <f>Generator4!C14</f>
+        <v>315.93876262626264</v>
+      </c>
+      <c r="C8" s="24">
+        <f>ABS(B7-B8)/B7</f>
+        <v>0.95770533876171648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>